<commit_message>
Added the weight table
</commit_message>
<xml_diff>
--- a/Inputs/outliers.xlsx
+++ b/Inputs/outliers.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\KUL\Master thesis\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B201B2DB-B8CC-493D-B20C-EE52F2122888}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA3D230-1EFA-440B-8BFD-36F56A7D08A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{6752877C-6E2E-466A-B1AE-08F695994F06}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{6752877C-6E2E-466A-B1AE-08F695994F06}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="table" sheetId="1" r:id="rId1"/>
+    <sheet name="weights" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="1003">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="1007">
   <si>
     <t>A_1_1</t>
   </si>
@@ -3039,6 +3040,18 @@
   </si>
   <si>
     <t>fallen seed</t>
+  </si>
+  <si>
+    <t>NOT_FG</t>
+  </si>
+  <si>
+    <t>LS weight</t>
+  </si>
+  <si>
+    <t>RS weight</t>
+  </si>
+  <si>
+    <t>Area</t>
   </si>
 </sst>
 </file>
@@ -3141,7 +3154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3150,6 +3163,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3466,9 +3481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1FF0D3-2C26-4360-8FBA-5A209FE02C7D}">
   <dimension ref="A1:I991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A752" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G772" sqref="G772"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="B1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11901,4 +11916,133 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DDE375-7B49-4C47-8224-F12876C3F35B}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>996</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>991</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>997</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.4</v>
+      </c>
+      <c r="D4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>992</v>
+      </c>
+      <c r="B5">
+        <v>0.8</v>
+      </c>
+      <c r="C5">
+        <v>0.8</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B7">
+        <v>0.8</v>
+      </c>
+      <c r="C7">
+        <v>0.8</v>
+      </c>
+      <c r="D7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>995</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code table for variables
</commit_message>
<xml_diff>
--- a/Inputs/outliers.xlsx
+++ b/Inputs/outliers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\KUL\Master thesis\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA3D230-1EFA-440B-8BFD-36F56A7D08A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B314764D-D51A-44B2-857D-3B620713E069}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{6752877C-6E2E-466A-B1AE-08F695994F06}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="1007">
   <si>
     <t>A_1_1</t>
   </si>
@@ -11922,9 +11922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DDE375-7B49-4C47-8224-F12876C3F35B}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11933,7 +11931,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8"/>
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" s="8" t="s">
         <v>1004</v>
       </c>

</xml_diff>